<commit_message>
score and rate companies
</commit_message>
<xml_diff>
--- a/2. preprocessing/dart/company_info.xlsx
+++ b/2. preprocessing/dart/company_info.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanah\Desktop\workspace\Project\ESG\2. preprocessing\dart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA678EC-4FF3-4FD6-86FC-D46ACA0FB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECC3798-8BD1-4336-BC04-CF08F317A558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -16754,14 +16757,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1218" workbookViewId="0">
-      <selection activeCell="M1223" sqref="M1223"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="N134" sqref="N134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12.09765625" customWidth="1"/>
     <col min="4" max="4" width="21.296875" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
@@ -56863,6 +56867,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>

</xml_diff>